<commit_message>
Added two new tasks: 1) init exceptions 2) dlog group new function: isIdentity
git-svn-id: https://svn.cs.biu.ac.il/svn/development/SDK@951 ba1fec17-5bc3-4c1d-a110-6a66ae20c876
</commit_message>
<xml_diff>
--- a/Docs/Miscelanous/TodoList.xlsx
+++ b/Docs/Miscelanous/TodoList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="98">
   <si>
     <t>Task name</t>
   </si>
@@ -529,6 +529,18 @@
   </si>
   <si>
     <t>In First Layer SDD: reconsider the PRF section</t>
+  </si>
+  <si>
+    <t>Init Exceptions</t>
+  </si>
+  <si>
+    <t>We should have a new exception called InitializationException that is thrown whenever the init function doesn't succeed. It collects the actual reason or exception why it didn't succeed and puts that as the message of the exception.</t>
+  </si>
+  <si>
+    <t>Dlog group-- isIdentity()</t>
+  </si>
+  <si>
+    <t>Add  a new function to DlogGroup interface: boolean isIdentity(GroupElement gEl)</t>
   </si>
 </sst>
 </file>
@@ -979,13 +991,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B47" sqref="B47"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1675,6 +1687,48 @@
       </c>
       <c r="D47" s="20"/>
       <c r="G47" s="20"/>
+    </row>
+    <row r="48" spans="1:7" s="22" customFormat="1" ht="30">
+      <c r="A48" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="23">
+        <v>40948</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G48" s="23"/>
+    </row>
+    <row r="49" spans="1:7" s="19" customFormat="1">
+      <c r="A49" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" s="20">
+        <v>40949</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G49" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added: where does Dlog group get source of randomness.
git-svn-id: https://svn.cs.biu.ac.il/svn/development/SDK@952 ba1fec17-5bc3-4c1d-a110-6a66ae20c876
</commit_message>
<xml_diff>
--- a/Docs/Miscelanous/TodoList.xlsx
+++ b/Docs/Miscelanous/TodoList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
   <si>
     <t>Task name</t>
   </si>
@@ -541,6 +541,12 @@
   </si>
   <si>
     <t>Add  a new function to DlogGroup interface: boolean isIdentity(GroupElement gEl)</t>
+  </si>
+  <si>
+    <t>Dlog group-- source of randomness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where should DlogGroup get the source of randomness from. At the moment, creates whenever needed new SecureRandom </t>
   </si>
 </sst>
 </file>
@@ -991,13 +997,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomRight" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1720,7 +1726,7 @@
         <v>97</v>
       </c>
       <c r="D49" s="20">
-        <v>40949</v>
+        <v>40948</v>
       </c>
       <c r="E49" s="19" t="s">
         <v>13</v>
@@ -1729,6 +1735,27 @@
         <v>78</v>
       </c>
       <c r="G49" s="20"/>
+    </row>
+    <row r="50" spans="1:7" s="22" customFormat="1">
+      <c r="A50" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" s="23">
+        <v>40948</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G50" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added: Need to do optimization of simultaneous exps in dlog.
git-svn-id: https://svn.cs.biu.ac.il/svn/development/SDK@990 ba1fec17-5bc3-4c1d-a110-6a66ae20c876
</commit_message>
<xml_diff>
--- a/Docs/Miscelanous/TodoList.xlsx
+++ b/Docs/Miscelanous/TodoList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
   <si>
     <t>Task name</t>
   </si>
@@ -547,6 +547,12 @@
   </si>
   <si>
     <t xml:space="preserve">Where should DlogGroup get the source of randomness from. At the moment, creates whenever needed new SecureRandom </t>
+  </si>
+  <si>
+    <t>DlogGroup-simultaneous exponentiations</t>
+  </si>
+  <si>
+    <t>This is not really a bug. At the moment we have implemented this function in a naïve way, without the optimization suggested in the book of applied crypto. See if we can optimize.</t>
   </si>
 </sst>
 </file>
@@ -997,13 +1003,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A41" sqref="A41"/>
+      <selection pane="bottomRight" activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1756,6 +1762,27 @@
         <v>78</v>
       </c>
       <c r="G50" s="23"/>
+    </row>
+    <row r="51" spans="1:7" s="19" customFormat="1" ht="30">
+      <c r="A51" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="20">
+        <v>40959</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G51" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. need to organize DlogGroup's init functions 2. need to organize TrapdoorPermutation's init functions
git-svn-id: https://svn.cs.biu.ac.il/svn/development/SDK@993 ba1fec17-5bc3-4c1d-a110-6a66ae20c876
</commit_message>
<xml_diff>
--- a/Docs/Miscelanous/TodoList.xlsx
+++ b/Docs/Miscelanous/TodoList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="110">
   <si>
     <t>Task name</t>
   </si>
@@ -553,6 +553,30 @@
   </si>
   <si>
     <t>This is not really a bug. At the moment we have implemented this function in a naïve way, without the optimization suggested in the book of applied crypto. See if we can optimize.</t>
+  </si>
+  <si>
+    <t>1. delete the init functions that gets a strings from elliptic curve classes. The init function that gets an algorithmParameterSpec does the same things.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. dlogZp - add a class DlogZpRandomParams that hold the numOfBits. </t>
+  </si>
+  <si>
+    <t>3. dlogZp - delete the init function that gets numOfBits. Instead,  the init function that gets the algorithmParameterSpec can get an instance of DlogZpRandomParams. IN this case this init function will act the same as the init that gets the numOfBits.</t>
+  </si>
+  <si>
+    <t>1. delete the init function that gets algorithmParameterSpec.</t>
+  </si>
+  <si>
+    <t>2. add  aclass KeyPairGenerator that gets the name of an algorithm and return a pair of keys to this algorithm. In case the name is Rabin - generate key pair using CryptoPpJavaInterface dll.</t>
+  </si>
+  <si>
+    <t>3.  the init function that gets the keys and an algorithmParameterSpec shouldn't throw an excetion, but ignore the params, as we did in other primitive families.</t>
+  </si>
+  <si>
+    <t>DlogGroup - init functions</t>
+  </si>
+  <si>
+    <t>TrapdoorPermutation - init functions</t>
   </si>
 </sst>
 </file>
@@ -1003,13 +1027,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A51" sqref="A51:XFD51"/>
+      <selection pane="bottomRight" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1783,6 +1807,72 @@
         <v>78</v>
       </c>
       <c r="G51" s="20"/>
+    </row>
+    <row r="52" spans="1:7" s="22" customFormat="1" ht="30">
+      <c r="A52" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D52" s="23">
+        <v>40965</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G52" s="23"/>
+    </row>
+    <row r="53" spans="1:7" s="22" customFormat="1">
+      <c r="A53" s="21"/>
+      <c r="C53" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" s="23"/>
+      <c r="G53" s="23"/>
+    </row>
+    <row r="54" spans="1:7" s="22" customFormat="1" ht="30">
+      <c r="A54" s="21"/>
+      <c r="C54" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="23"/>
+      <c r="G54" s="23"/>
+    </row>
+    <row r="55" spans="1:7" s="19" customFormat="1">
+      <c r="A55" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="20"/>
+      <c r="G55" s="20"/>
+    </row>
+    <row r="56" spans="1:7" s="19" customFormat="1" ht="30">
+      <c r="A56" s="18"/>
+      <c r="C56" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" s="20"/>
+      <c r="G56" s="20"/>
+    </row>
+    <row r="57" spans="1:7" s="19" customFormat="1" ht="30">
+      <c r="A57" s="18"/>
+      <c r="C57" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" s="20"/>
+      <c r="G57" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>